<commit_message>
Assigned self to task
</commit_message>
<xml_diff>
--- a/Documents/Plan for 18th December.xlsx
+++ b/Documents/Plan for 18th December.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Henry\Documents\GitHub\Notepad_Software\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\GitHub\Notepad_Software\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>To-Do List</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t>&gt; Once we have done these - is it worth doing another Sprint or not?</t>
+  </si>
+  <si>
+    <t>Alex</t>
   </si>
 </sst>
 </file>
@@ -210,11 +213,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -536,7 +539,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,13 +551,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="13">
+      <c r="A1" s="12">
         <v>42722</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="12"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
@@ -622,7 +625,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>7</v>

</xml_diff>